<commit_message>
update every type excel generate
重新更新所有分采购订单生成，更新订单信息，客户信息
普通，楦头，刀模，包材均采用不同函数生成
包材会自动将包装信息复制入采购订单内
更改了各种分尺码材料的显示方式
</commit_message>
<xml_diff>
--- a/backend-python/general_document/新标准采购订单尺码版.xlsx
+++ b/backend-python/general_document/新标准采购订单尺码版.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12255"/>
+    <workbookView windowWidth="28800" windowHeight="12375"/>
   </bookViews>
   <sheets>
     <sheet name="085" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>材料订购单</t>
   </si>
@@ -38,7 +38,10 @@
     <t>日期：</t>
   </si>
   <si>
-    <t>物品名称</t>
+    <t>型号</t>
+  </si>
+  <si>
+    <t>类别</t>
   </si>
   <si>
     <t xml:space="preserve"> 数量</t>
@@ -429,7 +432,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -476,17 +479,6 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -635,7 +627,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -647,34 +639,34 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -810,20 +802,20 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -841,31 +833,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1212,7 +1201,7 @@
   <dimension ref="A1:L60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1"/>
@@ -1262,646 +1251,648 @@
       <c r="H2" s="9"/>
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="18"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
     </row>
     <row r="3" customHeight="1" spans="1:12">
       <c r="A3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="14" t="s">
+      <c r="C3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="13" t="s">
         <v>6</v>
       </c>
+      <c r="L3" s="13" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" customHeight="1" spans="1:12">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="1:9">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7"/>
-      <c r="I7"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
     </row>
     <row r="8" customHeight="1" spans="1:9">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8"/>
-      <c r="I8"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
     </row>
     <row r="9" customHeight="1" spans="1:9">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9"/>
-      <c r="I9"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
     </row>
     <row r="10" customHeight="1" spans="1:9">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10"/>
-      <c r="I10"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
     </row>
     <row r="11" customHeight="1" spans="1:9">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11"/>
-      <c r="I11"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
     </row>
     <row r="12" customHeight="1" spans="1:9">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12"/>
-      <c r="I12"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
     </row>
     <row r="13" customHeight="1" spans="1:9">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13"/>
-      <c r="I13"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
     </row>
     <row r="14" customHeight="1" spans="1:9">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14"/>
-      <c r="I14"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
     </row>
     <row r="15" customHeight="1" spans="1:9">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15"/>
-      <c r="I15"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
     </row>
     <row r="16" s="2" customFormat="1" customHeight="1" spans="1:9">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16"/>
-      <c r="I16"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
     </row>
     <row r="17" s="2" customFormat="1" customHeight="1" spans="1:9">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17"/>
-      <c r="I17"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
     </row>
     <row r="18" s="2" customFormat="1" customHeight="1" spans="1:9">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18"/>
-      <c r="I18"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
     </row>
     <row r="19" customHeight="1" spans="1:9">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19"/>
-      <c r="I19"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
     </row>
     <row r="20" customHeight="1" spans="1:9">
-      <c r="A20" s="16"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20"/>
-      <c r="I20"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
     </row>
     <row r="21" s="1" customFormat="1" customHeight="1" spans="1:9">
-      <c r="A21" s="16"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21"/>
-      <c r="I21"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
     </row>
     <row r="22" customHeight="1" spans="1:9">
-      <c r="A22" s="16"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22"/>
-      <c r="I22"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
     </row>
     <row r="23" customHeight="1" spans="1:9">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23"/>
-      <c r="I23"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
     </row>
     <row r="24" customHeight="1" spans="1:9">
-      <c r="A24" s="16"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24"/>
-      <c r="I24"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
     </row>
     <row r="25" customHeight="1" spans="1:9">
-      <c r="A25" s="16"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25"/>
-      <c r="I25"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
     </row>
     <row r="26" customHeight="1" spans="1:9">
-      <c r="A26" s="16"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26"/>
-      <c r="I26"/>
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
     </row>
     <row r="27" customHeight="1" spans="1:9">
-      <c r="A27" s="16"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27"/>
-      <c r="I27"/>
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
     </row>
     <row r="28" customHeight="1" spans="1:9">
-      <c r="A28" s="16"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28"/>
-      <c r="I28"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
     </row>
     <row r="29" customHeight="1" spans="1:9">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29"/>
-      <c r="I29"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
     </row>
     <row r="30" s="2" customFormat="1" customHeight="1" spans="1:9">
-      <c r="A30" s="16"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30"/>
-      <c r="I30"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
     </row>
     <row r="31" s="2" customFormat="1" customHeight="1" spans="1:9">
-      <c r="A31" s="16"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31"/>
-      <c r="I31"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
     </row>
     <row r="32" s="2" customFormat="1" customHeight="1" spans="1:9">
-      <c r="A32" s="16"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
-      <c r="H32"/>
-      <c r="I32"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
     </row>
     <row r="33" customHeight="1" spans="1:9">
-      <c r="A33" s="16"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33"/>
-      <c r="I33"/>
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
     </row>
     <row r="34" customHeight="1" spans="1:9">
-      <c r="A34" s="16"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34"/>
-      <c r="I34"/>
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="1:9">
-      <c r="A35" s="16"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35"/>
-      <c r="I35"/>
+      <c r="A35" s="15"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
     </row>
     <row r="36" customHeight="1" spans="1:9">
-      <c r="A36" s="16"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
-      <c r="H36"/>
-      <c r="I36"/>
+      <c r="A36" s="15"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
     </row>
     <row r="37" customHeight="1" spans="1:9">
-      <c r="A37" s="16"/>
-      <c r="B37" s="16"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-      <c r="H37"/>
-      <c r="I37"/>
+      <c r="A37" s="15"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="16"/>
     </row>
     <row r="38" customHeight="1" spans="1:9">
-      <c r="A38" s="16"/>
-      <c r="B38" s="16"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38"/>
-      <c r="I38"/>
+      <c r="A38" s="15"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
     </row>
     <row r="39" customHeight="1" spans="1:9">
-      <c r="A39" s="16"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
-      <c r="H39"/>
-      <c r="I39"/>
+      <c r="A39" s="15"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
     </row>
     <row r="40" customHeight="1" spans="1:9">
-      <c r="A40" s="16"/>
-      <c r="B40" s="16"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="16"/>
-      <c r="G40" s="16"/>
-      <c r="H40"/>
-      <c r="I40"/>
+      <c r="A40" s="15"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16"/>
     </row>
     <row r="41" customHeight="1" spans="1:9">
-      <c r="A41" s="16"/>
-      <c r="B41" s="16"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
-      <c r="H41"/>
-      <c r="I41"/>
+      <c r="A41" s="15"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
     </row>
     <row r="42" customHeight="1" spans="1:9">
-      <c r="A42" s="16"/>
-      <c r="B42" s="16"/>
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="16"/>
-      <c r="H42"/>
-      <c r="I42"/>
+      <c r="A42" s="15"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
     </row>
     <row r="43" customHeight="1" spans="1:9">
-      <c r="A43" s="16"/>
-      <c r="B43" s="16"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
-      <c r="H43"/>
-      <c r="I43"/>
+      <c r="A43" s="15"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
     </row>
     <row r="44" s="2" customFormat="1" customHeight="1" spans="1:9">
-      <c r="A44" s="16"/>
-      <c r="B44" s="16"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="16"/>
-      <c r="H44"/>
-      <c r="I44"/>
+      <c r="A44" s="15"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="16"/>
     </row>
     <row r="45" s="2" customFormat="1" customHeight="1" spans="1:9">
-      <c r="A45" s="16"/>
-      <c r="B45" s="16"/>
-      <c r="C45" s="16"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="16"/>
-      <c r="H45"/>
-      <c r="I45"/>
+      <c r="A45" s="15"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
     </row>
     <row r="46" s="2" customFormat="1" customHeight="1" spans="1:9">
-      <c r="A46" s="16"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="16"/>
-      <c r="G46" s="16"/>
-      <c r="H46"/>
-      <c r="I46"/>
+      <c r="A46" s="15"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="16"/>
     </row>
     <row r="47" customHeight="1" spans="1:9">
-      <c r="A47" s="16"/>
-      <c r="B47" s="16"/>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
-      <c r="H47"/>
-      <c r="I47"/>
+      <c r="A47" s="15"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
     </row>
     <row r="48" customHeight="1" spans="1:9">
-      <c r="A48" s="16"/>
-      <c r="B48" s="16"/>
-      <c r="C48" s="16"/>
-      <c r="D48" s="16"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="16"/>
-      <c r="G48" s="16"/>
-      <c r="H48"/>
-      <c r="I48"/>
+      <c r="A48" s="15"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="16"/>
+      <c r="I48" s="16"/>
     </row>
     <row r="49" s="1" customFormat="1" customHeight="1" spans="1:9">
-      <c r="A49" s="16"/>
-      <c r="B49" s="16"/>
-      <c r="C49" s="16"/>
-      <c r="D49" s="16"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="16"/>
-      <c r="G49" s="16"/>
-      <c r="H49"/>
-      <c r="I49"/>
+      <c r="A49" s="15"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="16"/>
+      <c r="I49" s="16"/>
     </row>
     <row r="50" customHeight="1" spans="1:9">
-      <c r="A50" s="16"/>
-      <c r="B50" s="16"/>
-      <c r="C50" s="16"/>
-      <c r="D50" s="16"/>
-      <c r="E50" s="16"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="16"/>
-      <c r="H50"/>
-      <c r="I50"/>
+      <c r="A50" s="15"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="16"/>
+      <c r="I50" s="16"/>
     </row>
     <row r="51" customHeight="1" spans="1:9">
-      <c r="A51" s="16"/>
-      <c r="B51" s="16"/>
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="16"/>
-      <c r="G51" s="16"/>
-      <c r="H51"/>
-      <c r="I51"/>
+      <c r="A51" s="15"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="16"/>
+      <c r="I51" s="16"/>
     </row>
     <row r="52" customHeight="1" spans="1:9">
-      <c r="A52" s="16"/>
-      <c r="B52" s="16"/>
-      <c r="C52" s="16"/>
-      <c r="D52" s="16"/>
-      <c r="E52" s="16"/>
-      <c r="F52" s="16"/>
-      <c r="G52" s="16"/>
-      <c r="H52"/>
-      <c r="I52"/>
+      <c r="A52" s="15"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="16"/>
+      <c r="I52" s="16"/>
     </row>
     <row r="53" customHeight="1" spans="1:9">
-      <c r="A53" s="16"/>
-      <c r="B53" s="16"/>
-      <c r="C53" s="16"/>
-      <c r="D53" s="16"/>
-      <c r="E53" s="16"/>
-      <c r="F53" s="16"/>
-      <c r="G53" s="16"/>
-      <c r="H53"/>
-      <c r="I53"/>
+      <c r="A53" s="15"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="16"/>
+      <c r="I53" s="16"/>
     </row>
     <row r="54" customHeight="1" spans="1:9">
-      <c r="A54" s="16"/>
-      <c r="B54" s="16"/>
-      <c r="C54" s="16"/>
-      <c r="D54" s="16"/>
-      <c r="E54" s="16"/>
-      <c r="F54" s="16"/>
-      <c r="G54" s="16"/>
-      <c r="H54"/>
-      <c r="I54"/>
+      <c r="A54" s="15"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="16"/>
+      <c r="I54" s="16"/>
     </row>
     <row r="55" customHeight="1" spans="1:9">
-      <c r="A55" s="16"/>
-      <c r="B55" s="16"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="16"/>
-      <c r="F55" s="16"/>
-      <c r="G55" s="16"/>
-      <c r="H55"/>
-      <c r="I55"/>
+      <c r="A55" s="15"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="16"/>
+      <c r="I55" s="16"/>
     </row>
     <row r="56" customHeight="1" spans="1:9">
-      <c r="A56" s="16"/>
-      <c r="B56" s="16"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="16"/>
-      <c r="G56" s="16"/>
-      <c r="H56"/>
-      <c r="I56"/>
+      <c r="A56" s="15"/>
+      <c r="B56" s="15"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="15"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="16"/>
+      <c r="I56" s="16"/>
     </row>
     <row r="57" customHeight="1" spans="1:9">
-      <c r="A57" s="16"/>
-      <c r="B57" s="16"/>
-      <c r="C57" s="16"/>
-      <c r="D57" s="16"/>
-      <c r="E57" s="16"/>
-      <c r="F57" s="16"/>
-      <c r="G57" s="16"/>
-      <c r="H57"/>
-      <c r="I57"/>
+      <c r="A57" s="15"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="16"/>
+      <c r="I57" s="16"/>
     </row>
     <row r="58" s="2" customFormat="1" customHeight="1" spans="1:9">
-      <c r="A58" s="16"/>
-      <c r="B58" s="16"/>
-      <c r="C58" s="16"/>
-      <c r="D58" s="16"/>
-      <c r="E58" s="16"/>
-      <c r="F58" s="16"/>
-      <c r="G58" s="16"/>
-      <c r="H58"/>
-      <c r="I58"/>
+      <c r="A58" s="15"/>
+      <c r="B58" s="15"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="16"/>
+      <c r="I58" s="16"/>
     </row>
     <row r="59" s="2" customFormat="1" customHeight="1" spans="1:9">
-      <c r="A59" s="16"/>
-      <c r="B59" s="16"/>
-      <c r="C59" s="16"/>
-      <c r="D59" s="16"/>
-      <c r="E59" s="16"/>
-      <c r="F59" s="16"/>
-      <c r="G59" s="16"/>
-      <c r="H59"/>
-      <c r="I59"/>
+      <c r="A59" s="15"/>
+      <c r="B59" s="15"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="16"/>
+      <c r="I59" s="16"/>
     </row>
     <row r="60" s="2" customFormat="1" customHeight="1" spans="1:9">
-      <c r="A60" s="16"/>
-      <c r="B60" s="16"/>
-      <c r="C60" s="16"/>
-      <c r="D60" s="16"/>
-      <c r="E60" s="16"/>
-      <c r="F60" s="16"/>
-      <c r="G60" s="16"/>
-      <c r="H60"/>
-      <c r="I60"/>
+      <c r="A60" s="15"/>
+      <c r="B60" s="15"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="15"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="16"/>
+      <c r="I60" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:L2"/>
     <mergeCell ref="C3:J3"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>

</xml_diff>